<commit_message>
Update - Version 0.6
- changed the work mode of the CU from simple to complex
- added full support for Instruments ( working properly )
- Excel from Customize tab should match the generated Excel when using the characterization function

#TODO&FIX
- DeviceControlLib method GetAllConections interferences the Remote Instrumentations with other USB/Bluetooth connections such as Headphones.
</commit_message>
<xml_diff>
--- a/PCU GUI Idea/Excel Templates/Excel Data/template.xlsx
+++ b/PCU GUI Idea/Excel Templates/Excel Data/template.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bogdan\Documents\GitHub\PCU-12V-12V-1.2kW\PCU GUI Idea\Excel Templates\Excel Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DBF63B94-B4AE-4CAC-BBE6-A64DD8FDEC98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{413D505E-9394-4E2E-9275-16CA8DB9B00A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="720" windowWidth="21600" windowHeight="12735" xr2:uid="{59DB622C-15EC-4E72-98EC-A9F5CDA0BF36}"/>
+    <workbookView xWindow="3780" yWindow="-16215" windowWidth="21600" windowHeight="11385" xr2:uid="{58EDFBF6-7758-474E-B338-2B6862006E1F}"/>
   </bookViews>
   <sheets>
-    <sheet name="25-02-2025 15-15" sheetId="1" r:id="rId1"/>
+    <sheet name="04-03-2025 14-11" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -628,17 +628,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4637C210-3309-490F-8A38-E606D95190A4}">
-  <dimension ref="B2:U35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F48F1DF6-1319-426A-B6FC-5712CD3A8DEB}">
+  <dimension ref="B2:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:21" ht="21" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:11" ht="21" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -650,14 +650,14 @@
       </c>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="2:21" ht="21" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:11" ht="21" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="G3" s="3"/>
     </row>
-    <row r="5" spans="2:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
@@ -685,41 +685,11 @@
       <c r="J5" s="6">
         <v>450</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K5" s="7">
         <v>500</v>
       </c>
-      <c r="L5" s="6">
-        <v>550</v>
-      </c>
-      <c r="M5" s="6">
-        <v>600</v>
-      </c>
-      <c r="N5" s="6">
-        <v>650</v>
-      </c>
-      <c r="O5" s="6">
-        <v>700</v>
-      </c>
-      <c r="P5" s="6">
-        <v>750</v>
-      </c>
-      <c r="Q5" s="6">
-        <v>800</v>
-      </c>
-      <c r="R5" s="6">
-        <v>850</v>
-      </c>
-      <c r="S5" s="6">
-        <v>900</v>
-      </c>
-      <c r="T5" s="6">
-        <v>950</v>
-      </c>
-      <c r="U5" s="7">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="8">
         <v>1</v>
       </c>
@@ -731,19 +701,9 @@
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="12"/>
-      <c r="R6" s="12"/>
-      <c r="S6" s="12"/>
-      <c r="T6" s="12"/>
-      <c r="U6" s="17"/>
-    </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="K6" s="17"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="9">
         <v>2</v>
       </c>
@@ -755,19 +715,9 @@
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
       <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="14"/>
-      <c r="S7" s="14"/>
-      <c r="T7" s="14"/>
-      <c r="U7" s="18"/>
-    </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="K7" s="18"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="9">
         <v>3</v>
       </c>
@@ -779,19 +729,9 @@
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
       <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="14"/>
-      <c r="Q8" s="14"/>
-      <c r="R8" s="14"/>
-      <c r="S8" s="14"/>
-      <c r="T8" s="14"/>
-      <c r="U8" s="18"/>
-    </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="K8" s="18"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="9">
         <v>4</v>
       </c>
@@ -803,19 +743,9 @@
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="14"/>
-      <c r="P9" s="14"/>
-      <c r="Q9" s="14"/>
-      <c r="R9" s="14"/>
-      <c r="S9" s="14"/>
-      <c r="T9" s="14"/>
-      <c r="U9" s="18"/>
-    </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="K9" s="18"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="9">
         <v>5</v>
       </c>
@@ -827,19 +757,9 @@
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="14"/>
-      <c r="P10" s="14"/>
-      <c r="Q10" s="14"/>
-      <c r="R10" s="14"/>
-      <c r="S10" s="14"/>
-      <c r="T10" s="14"/>
-      <c r="U10" s="18"/>
-    </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="K10" s="18"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="9">
         <v>6</v>
       </c>
@@ -851,19 +771,9 @@
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="14"/>
-      <c r="P11" s="14"/>
-      <c r="Q11" s="14"/>
-      <c r="R11" s="14"/>
-      <c r="S11" s="14"/>
-      <c r="T11" s="14"/>
-      <c r="U11" s="18"/>
-    </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="K11" s="18"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="9">
         <v>7</v>
       </c>
@@ -875,19 +785,9 @@
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
-      <c r="P12" s="14"/>
-      <c r="Q12" s="14"/>
-      <c r="R12" s="14"/>
-      <c r="S12" s="14"/>
-      <c r="T12" s="14"/>
-      <c r="U12" s="18"/>
-    </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="K12" s="18"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="9">
         <v>8</v>
       </c>
@@ -899,19 +799,9 @@
       <c r="H13" s="14"/>
       <c r="I13" s="14"/>
       <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
-      <c r="P13" s="14"/>
-      <c r="Q13" s="14"/>
-      <c r="R13" s="14"/>
-      <c r="S13" s="14"/>
-      <c r="T13" s="14"/>
-      <c r="U13" s="18"/>
-    </row>
-    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="K13" s="18"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="9">
         <v>9</v>
       </c>
@@ -923,19 +813,9 @@
       <c r="H14" s="14"/>
       <c r="I14" s="14"/>
       <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
-      <c r="P14" s="14"/>
-      <c r="Q14" s="14"/>
-      <c r="R14" s="14"/>
-      <c r="S14" s="14"/>
-      <c r="T14" s="14"/>
-      <c r="U14" s="18"/>
-    </row>
-    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="K14" s="18"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="9">
         <v>10</v>
       </c>
@@ -947,19 +827,9 @@
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
       <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="14"/>
-      <c r="Q15" s="14"/>
-      <c r="R15" s="14"/>
-      <c r="S15" s="14"/>
-      <c r="T15" s="14"/>
-      <c r="U15" s="18"/>
-    </row>
-    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="K15" s="18"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="9">
         <v>11</v>
       </c>
@@ -971,19 +841,9 @@
       <c r="H16" s="14"/>
       <c r="I16" s="14"/>
       <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14"/>
-      <c r="P16" s="14"/>
-      <c r="Q16" s="14"/>
-      <c r="R16" s="14"/>
-      <c r="S16" s="14"/>
-      <c r="T16" s="14"/>
-      <c r="U16" s="18"/>
-    </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="K16" s="18"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="9">
         <v>12</v>
       </c>
@@ -995,19 +855,9 @@
       <c r="H17" s="14"/>
       <c r="I17" s="14"/>
       <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
-      <c r="N17" s="14"/>
-      <c r="O17" s="14"/>
-      <c r="P17" s="14"/>
-      <c r="Q17" s="14"/>
-      <c r="R17" s="14"/>
-      <c r="S17" s="14"/>
-      <c r="T17" s="14"/>
-      <c r="U17" s="18"/>
-    </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="K17" s="18"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="9">
         <v>13</v>
       </c>
@@ -1019,19 +869,9 @@
       <c r="H18" s="14"/>
       <c r="I18" s="14"/>
       <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="14"/>
-      <c r="O18" s="14"/>
-      <c r="P18" s="14"/>
-      <c r="Q18" s="14"/>
-      <c r="R18" s="14"/>
-      <c r="S18" s="14"/>
-      <c r="T18" s="14"/>
-      <c r="U18" s="18"/>
-    </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="K18" s="18"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="9">
         <v>14</v>
       </c>
@@ -1043,19 +883,9 @@
       <c r="H19" s="14"/>
       <c r="I19" s="14"/>
       <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="14"/>
-      <c r="O19" s="14"/>
-      <c r="P19" s="14"/>
-      <c r="Q19" s="14"/>
-      <c r="R19" s="14"/>
-      <c r="S19" s="14"/>
-      <c r="T19" s="14"/>
-      <c r="U19" s="18"/>
-    </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="K19" s="18"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="9">
         <v>15</v>
       </c>
@@ -1067,19 +897,9 @@
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
       <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="14"/>
-      <c r="O20" s="14"/>
-      <c r="P20" s="14"/>
-      <c r="Q20" s="14"/>
-      <c r="R20" s="14"/>
-      <c r="S20" s="14"/>
-      <c r="T20" s="14"/>
-      <c r="U20" s="18"/>
-    </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="K20" s="18"/>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="9">
         <v>16</v>
       </c>
@@ -1091,19 +911,9 @@
       <c r="H21" s="14"/>
       <c r="I21" s="14"/>
       <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="14"/>
-      <c r="O21" s="14"/>
-      <c r="P21" s="14"/>
-      <c r="Q21" s="14"/>
-      <c r="R21" s="14"/>
-      <c r="S21" s="14"/>
-      <c r="T21" s="14"/>
-      <c r="U21" s="18"/>
-    </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="K21" s="18"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" s="9">
         <v>17</v>
       </c>
@@ -1115,19 +925,9 @@
       <c r="H22" s="14"/>
       <c r="I22" s="14"/>
       <c r="J22" s="14"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="14"/>
-      <c r="N22" s="14"/>
-      <c r="O22" s="14"/>
-      <c r="P22" s="14"/>
-      <c r="Q22" s="14"/>
-      <c r="R22" s="14"/>
-      <c r="S22" s="14"/>
-      <c r="T22" s="14"/>
-      <c r="U22" s="18"/>
-    </row>
-    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="K22" s="18"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="9">
         <v>18</v>
       </c>
@@ -1139,19 +939,9 @@
       <c r="H23" s="14"/>
       <c r="I23" s="14"/>
       <c r="J23" s="14"/>
-      <c r="K23" s="14"/>
-      <c r="L23" s="14"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="14"/>
-      <c r="O23" s="14"/>
-      <c r="P23" s="14"/>
-      <c r="Q23" s="14"/>
-      <c r="R23" s="14"/>
-      <c r="S23" s="14"/>
-      <c r="T23" s="14"/>
-      <c r="U23" s="18"/>
-    </row>
-    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="K23" s="18"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="9">
         <v>19</v>
       </c>
@@ -1163,288 +953,28 @@
       <c r="H24" s="14"/>
       <c r="I24" s="14"/>
       <c r="J24" s="14"/>
-      <c r="K24" s="14"/>
-      <c r="L24" s="14"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="14"/>
-      <c r="O24" s="14"/>
-      <c r="P24" s="14"/>
-      <c r="Q24" s="14"/>
-      <c r="R24" s="14"/>
-      <c r="S24" s="14"/>
-      <c r="T24" s="14"/>
-      <c r="U24" s="18"/>
-    </row>
-    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B25" s="9">
+      <c r="K24" s="18"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="10">
         <v>20</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="14"/>
-      <c r="K25" s="14"/>
-      <c r="L25" s="14"/>
-      <c r="M25" s="14"/>
-      <c r="N25" s="14"/>
-      <c r="O25" s="14"/>
-      <c r="P25" s="14"/>
-      <c r="Q25" s="14"/>
-      <c r="R25" s="14"/>
-      <c r="S25" s="14"/>
-      <c r="T25" s="14"/>
-      <c r="U25" s="18"/>
-    </row>
-    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B26" s="9">
-        <v>21</v>
-      </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="14"/>
-      <c r="K26" s="14"/>
-      <c r="L26" s="14"/>
-      <c r="M26" s="14"/>
-      <c r="N26" s="14"/>
-      <c r="O26" s="14"/>
-      <c r="P26" s="14"/>
-      <c r="Q26" s="14"/>
-      <c r="R26" s="14"/>
-      <c r="S26" s="14"/>
-      <c r="T26" s="14"/>
-      <c r="U26" s="18"/>
-    </row>
-    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B27" s="9">
-        <v>22</v>
-      </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
-      <c r="K27" s="14"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="14"/>
-      <c r="N27" s="14"/>
-      <c r="O27" s="14"/>
-      <c r="P27" s="14"/>
-      <c r="Q27" s="14"/>
-      <c r="R27" s="14"/>
-      <c r="S27" s="14"/>
-      <c r="T27" s="14"/>
-      <c r="U27" s="18"/>
-    </row>
-    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B28" s="9">
-        <v>23</v>
-      </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="14"/>
-      <c r="K28" s="14"/>
-      <c r="L28" s="14"/>
-      <c r="M28" s="14"/>
-      <c r="N28" s="14"/>
-      <c r="O28" s="14"/>
-      <c r="P28" s="14"/>
-      <c r="Q28" s="14"/>
-      <c r="R28" s="14"/>
-      <c r="S28" s="14"/>
-      <c r="T28" s="14"/>
-      <c r="U28" s="18"/>
-    </row>
-    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B29" s="9">
-        <v>24</v>
-      </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="14"/>
-      <c r="K29" s="14"/>
-      <c r="L29" s="14"/>
-      <c r="M29" s="14"/>
-      <c r="N29" s="14"/>
-      <c r="O29" s="14"/>
-      <c r="P29" s="14"/>
-      <c r="Q29" s="14"/>
-      <c r="R29" s="14"/>
-      <c r="S29" s="14"/>
-      <c r="T29" s="14"/>
-      <c r="U29" s="18"/>
-    </row>
-    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B30" s="9">
-        <v>25</v>
-      </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="14"/>
-      <c r="K30" s="14"/>
-      <c r="L30" s="14"/>
-      <c r="M30" s="14"/>
-      <c r="N30" s="14"/>
-      <c r="O30" s="14"/>
-      <c r="P30" s="14"/>
-      <c r="Q30" s="14"/>
-      <c r="R30" s="14"/>
-      <c r="S30" s="14"/>
-      <c r="T30" s="14"/>
-      <c r="U30" s="18"/>
-    </row>
-    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B31" s="9">
-        <v>26</v>
-      </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="14"/>
-      <c r="J31" s="14"/>
-      <c r="K31" s="14"/>
-      <c r="L31" s="14"/>
-      <c r="M31" s="14"/>
-      <c r="N31" s="14"/>
-      <c r="O31" s="14"/>
-      <c r="P31" s="14"/>
-      <c r="Q31" s="14"/>
-      <c r="R31" s="14"/>
-      <c r="S31" s="14"/>
-      <c r="T31" s="14"/>
-      <c r="U31" s="18"/>
-    </row>
-    <row r="32" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B32" s="9">
-        <v>27</v>
-      </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="14"/>
-      <c r="J32" s="14"/>
-      <c r="K32" s="14"/>
-      <c r="L32" s="14"/>
-      <c r="M32" s="14"/>
-      <c r="N32" s="14"/>
-      <c r="O32" s="14"/>
-      <c r="P32" s="14"/>
-      <c r="Q32" s="14"/>
-      <c r="R32" s="14"/>
-      <c r="S32" s="14"/>
-      <c r="T32" s="14"/>
-      <c r="U32" s="18"/>
-    </row>
-    <row r="33" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B33" s="9">
-        <v>28</v>
-      </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="14"/>
-      <c r="J33" s="14"/>
-      <c r="K33" s="14"/>
-      <c r="L33" s="14"/>
-      <c r="M33" s="14"/>
-      <c r="N33" s="14"/>
-      <c r="O33" s="14"/>
-      <c r="P33" s="14"/>
-      <c r="Q33" s="14"/>
-      <c r="R33" s="14"/>
-      <c r="S33" s="14"/>
-      <c r="T33" s="14"/>
-      <c r="U33" s="18"/>
-    </row>
-    <row r="34" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B34" s="9">
-        <v>29</v>
-      </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14"/>
-      <c r="I34" s="14"/>
-      <c r="J34" s="14"/>
-      <c r="K34" s="14"/>
-      <c r="L34" s="14"/>
-      <c r="M34" s="14"/>
-      <c r="N34" s="14"/>
-      <c r="O34" s="14"/>
-      <c r="P34" s="14"/>
-      <c r="Q34" s="14"/>
-      <c r="R34" s="14"/>
-      <c r="S34" s="14"/>
-      <c r="T34" s="14"/>
-      <c r="U34" s="18"/>
-    </row>
-    <row r="35" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B35" s="10">
-        <v>30</v>
-      </c>
-      <c r="C35" s="15"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="16"/>
-      <c r="H35" s="16"/>
-      <c r="I35" s="16"/>
-      <c r="J35" s="16"/>
-      <c r="K35" s="16"/>
-      <c r="L35" s="16"/>
-      <c r="M35" s="16"/>
-      <c r="N35" s="16"/>
-      <c r="O35" s="16"/>
-      <c r="P35" s="16"/>
-      <c r="Q35" s="16"/>
-      <c r="R35" s="16"/>
-      <c r="S35" s="16"/>
-      <c r="T35" s="16"/>
-      <c r="U35" s="19"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B2:E3"/>
     <mergeCell ref="G2:H2"/>
   </mergeCells>
-  <conditionalFormatting sqref="C5:U5">
+  <conditionalFormatting sqref="C5:K5">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -1454,7 +984,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6:B35">
+  <conditionalFormatting sqref="B6:B25">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -1464,7 +994,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C6:U35">
+  <conditionalFormatting sqref="C6:K25">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>